<commit_message>
Fixed incorrect hours calculation
</commit_message>
<xml_diff>
--- a/WinGUI/Assets/template_pion.xlsx
+++ b/WinGUI/Assets/template_pion.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Source\Repos\VF Raporty Godzin Pracy\WinGUI\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\RescueRangers\VF-Raporty-godzin-pracy\WinGUI\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5518332-54BB-440B-88DD-25D611FE7B24}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9060"/>
+    <workbookView xWindow="28680" yWindow="1620" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,13 +155,7 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -175,6 +170,8 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,17 +485,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
@@ -506,20 +503,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -529,11 +526,11 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -562,236 +559,236 @@
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="2"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
     </row>
     <row r="45" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="14"/>
+      <c r="E45" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>